<commit_message>
added hdmf, philhealth table
</commit_message>
<xml_diff>
--- a/assets/new template.xlsx
+++ b/assets/new template.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Romel\Desktop\Desktop Files\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule Infor." sheetId="1" r:id="rId1"/>
@@ -17,7 +12,7 @@
     <sheet name="Att.log report" sheetId="3" r:id="rId3"/>
     <sheet name="Exception Stat." sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -372,10 +367,10 @@
     <t>2020-10-27</t>
   </si>
   <si>
-    <t>00001-A</t>
-  </si>
-  <si>
-    <t>00004-A</t>
+    <t>00008-A</t>
+  </si>
+  <si>
+    <t>00014-A</t>
   </si>
 </sst>
 </file>
@@ -383,7 +378,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -958,6 +953,9 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="8"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="8"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1026,9 +1024,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="16" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -1098,7 +1093,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1133,7 +1128,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1310,7 +1305,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1331,41 +1326,41 @@
   <sheetData>
     <row r="1" spans="1:34" ht="30">
       <c r="A1" s="1"/>
-      <c r="B1" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
-      <c r="T1" s="46"/>
-      <c r="U1" s="46"/>
-      <c r="V1" s="46"/>
-      <c r="W1" s="46"/>
-      <c r="X1" s="47"/>
-      <c r="Y1" s="47"/>
-      <c r="Z1" s="47"/>
-      <c r="AA1" s="47"/>
-      <c r="AB1" s="47"/>
-      <c r="AC1" s="47"/>
-      <c r="AD1" s="47"/>
-      <c r="AE1" s="47"/>
-      <c r="AF1" s="47"/>
-      <c r="AG1" s="47"/>
-      <c r="AH1" s="48"/>
+      <c r="B1" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="48"/>
+      <c r="Y1" s="48"/>
+      <c r="Z1" s="48"/>
+      <c r="AA1" s="48"/>
+      <c r="AB1" s="48"/>
+      <c r="AC1" s="48"/>
+      <c r="AD1" s="48"/>
+      <c r="AE1" s="48"/>
+      <c r="AF1" s="48"/>
+      <c r="AG1" s="48"/>
+      <c r="AH1" s="49"/>
     </row>
     <row r="2" spans="1:34">
       <c r="A2" s="2" t="s">
@@ -1389,34 +1384,34 @@
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
-      <c r="R2" s="49" t="s">
+      <c r="R2" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="S2" s="49"/>
-      <c r="T2" s="49"/>
-      <c r="U2" s="49"/>
-      <c r="V2" s="49"/>
-      <c r="W2" s="49"/>
-      <c r="X2" s="49"/>
-      <c r="Y2" s="49"/>
-      <c r="Z2" s="49"/>
-      <c r="AA2" s="49"/>
-      <c r="AB2" s="49"/>
-      <c r="AC2" s="49"/>
-      <c r="AD2" s="49"/>
-      <c r="AE2" s="49"/>
-      <c r="AF2" s="49"/>
-      <c r="AG2" s="49"/>
-      <c r="AH2" s="50"/>
+      <c r="S2" s="50"/>
+      <c r="T2" s="50"/>
+      <c r="U2" s="50"/>
+      <c r="V2" s="50"/>
+      <c r="W2" s="50"/>
+      <c r="X2" s="50"/>
+      <c r="Y2" s="50"/>
+      <c r="Z2" s="50"/>
+      <c r="AA2" s="50"/>
+      <c r="AB2" s="50"/>
+      <c r="AC2" s="50"/>
+      <c r="AD2" s="50"/>
+      <c r="AE2" s="50"/>
+      <c r="AF2" s="50"/>
+      <c r="AG2" s="50"/>
+      <c r="AH2" s="51"/>
     </row>
     <row r="3" spans="1:34" ht="15" customHeight="1">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="52" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="5">
@@ -1508,9 +1503,9 @@
       <c r="AH3" s="5"/>
     </row>
     <row r="4" spans="1:34">
-      <c r="A4" s="52"/>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
+      <c r="A4" s="53"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
       <c r="D4" s="6" t="s">
         <v>7</v>
       </c>
@@ -1986,31 +1981,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="30">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="V1" s="56"/>
-      <c r="W1" s="57"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="W1" s="58"/>
     </row>
     <row r="2" spans="1:23" ht="30">
       <c r="A2" s="9" t="s">
@@ -2042,64 +2037,64 @@
       <c r="W2" s="15"/>
     </row>
     <row r="3" spans="1:23">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="58" t="s">
+      <c r="D3" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="59"/>
-      <c r="F3" s="54" t="s">
+      <c r="E3" s="60"/>
+      <c r="F3" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54" t="s">
+      <c r="G3" s="55"/>
+      <c r="H3" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54" t="s">
+      <c r="I3" s="55"/>
+      <c r="J3" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54" t="s">
+      <c r="K3" s="55"/>
+      <c r="L3" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="M3" s="54" t="s">
+      <c r="M3" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="N3" s="54" t="s">
+      <c r="N3" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="O3" s="54" t="s">
+      <c r="O3" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="P3" s="54" t="s">
+      <c r="P3" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="Q3" s="54"/>
-      <c r="R3" s="54"/>
-      <c r="S3" s="54" t="s">
+      <c r="Q3" s="55"/>
+      <c r="R3" s="55"/>
+      <c r="S3" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="T3" s="54"/>
-      <c r="U3" s="54"/>
-      <c r="V3" s="54" t="s">
+      <c r="T3" s="55"/>
+      <c r="U3" s="55"/>
+      <c r="V3" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="W3" s="54" t="s">
+      <c r="W3" s="55" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:23">
-      <c r="A4" s="58"/>
-      <c r="B4" s="58"/>
-      <c r="C4" s="58"/>
+      <c r="A4" s="59"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
       <c r="D4" s="16" t="s">
         <v>36</v>
       </c>
@@ -2124,10 +2119,10 @@
       <c r="K4" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="L4" s="54"/>
-      <c r="M4" s="54"/>
-      <c r="N4" s="54"/>
-      <c r="O4" s="54"/>
+      <c r="L4" s="55"/>
+      <c r="M4" s="55"/>
+      <c r="N4" s="55"/>
+      <c r="O4" s="55"/>
       <c r="P4" s="18" t="s">
         <v>42</v>
       </c>
@@ -2146,8 +2141,8 @@
       <c r="U4" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="V4" s="54"/>
-      <c r="W4" s="54"/>
+      <c r="V4" s="55"/>
+      <c r="W4" s="55"/>
     </row>
     <row r="5" spans="1:23">
       <c r="A5" s="19" t="s">
@@ -2410,72 +2405,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="61"/>
-      <c r="P1" s="61"/>
-      <c r="Q1" s="61"/>
-      <c r="R1" s="61"/>
-      <c r="S1" s="61"/>
-      <c r="T1" s="61"/>
-      <c r="U1" s="61"/>
-      <c r="V1" s="61"/>
-      <c r="W1" s="61"/>
-      <c r="X1" s="61"/>
-      <c r="Y1" s="61"/>
-      <c r="Z1" s="61"/>
-      <c r="AA1" s="61"/>
-      <c r="AB1" s="61"/>
-      <c r="AC1" s="61"/>
-      <c r="AD1" s="61"/>
-      <c r="AE1" s="62"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="62"/>
+      <c r="Q1" s="62"/>
+      <c r="R1" s="62"/>
+      <c r="S1" s="62"/>
+      <c r="T1" s="62"/>
+      <c r="U1" s="62"/>
+      <c r="V1" s="62"/>
+      <c r="W1" s="62"/>
+      <c r="X1" s="62"/>
+      <c r="Y1" s="62"/>
+      <c r="Z1" s="62"/>
+      <c r="AA1" s="62"/>
+      <c r="AB1" s="62"/>
+      <c r="AC1" s="62"/>
+      <c r="AD1" s="62"/>
+      <c r="AE1" s="63"/>
     </row>
     <row r="2" spans="1:31">
-      <c r="A2" s="63"/>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64"/>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64"/>
-      <c r="Q2" s="64"/>
-      <c r="R2" s="64"/>
-      <c r="S2" s="64"/>
-      <c r="T2" s="64"/>
-      <c r="U2" s="64"/>
-      <c r="V2" s="64"/>
-      <c r="W2" s="64"/>
-      <c r="X2" s="64"/>
-      <c r="Y2" s="64"/>
-      <c r="Z2" s="64"/>
-      <c r="AA2" s="64"/>
-      <c r="AB2" s="64"/>
-      <c r="AC2" s="64"/>
-      <c r="AD2" s="64"/>
-      <c r="AE2" s="65"/>
+      <c r="A2" s="64"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="65"/>
+      <c r="N2" s="65"/>
+      <c r="O2" s="65"/>
+      <c r="P2" s="65"/>
+      <c r="Q2" s="65"/>
+      <c r="R2" s="65"/>
+      <c r="S2" s="65"/>
+      <c r="T2" s="65"/>
+      <c r="U2" s="65"/>
+      <c r="V2" s="65"/>
+      <c r="W2" s="65"/>
+      <c r="X2" s="65"/>
+      <c r="Y2" s="65"/>
+      <c r="Z2" s="65"/>
+      <c r="AA2" s="65"/>
+      <c r="AB2" s="65"/>
+      <c r="AC2" s="65"/>
+      <c r="AD2" s="65"/>
+      <c r="AE2" s="66"/>
     </row>
     <row r="3" spans="1:31">
       <c r="A3" s="23" t="s">
@@ -2510,13 +2505,13 @@
       <c r="V3" s="24"/>
       <c r="W3" s="24"/>
       <c r="X3" s="10"/>
-      <c r="Y3" s="66"/>
-      <c r="Z3" s="66"/>
-      <c r="AA3" s="66"/>
-      <c r="AB3" s="66"/>
-      <c r="AC3" s="66"/>
-      <c r="AD3" s="66"/>
-      <c r="AE3" s="67"/>
+      <c r="Y3" s="67"/>
+      <c r="Z3" s="67"/>
+      <c r="AA3" s="67"/>
+      <c r="AB3" s="67"/>
+      <c r="AC3" s="67"/>
+      <c r="AD3" s="67"/>
+      <c r="AE3" s="68"/>
     </row>
     <row r="4" spans="1:31">
       <c r="A4" s="25">
@@ -2976,8 +2971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H50" sqref="H50"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54:A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
@@ -2987,21 +2982,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="30">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="57"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="58"/>
     </row>
     <row r="2" spans="1:13" ht="30">
       <c r="A2" s="30" t="s">
@@ -3023,47 +3018,47 @@
       <c r="M2" s="36"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="68" t="s">
+      <c r="A3" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="68" t="s">
+      <c r="D3" s="69" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="54" t="s">
+      <c r="E3" s="55" t="s">
         <v>83</v>
       </c>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54" t="s">
+      <c r="F3" s="55"/>
+      <c r="G3" s="55" t="s">
         <v>84</v>
       </c>
-      <c r="H3" s="54"/>
-      <c r="I3" s="68" t="s">
+      <c r="H3" s="55"/>
+      <c r="I3" s="69" t="s">
         <v>85</v>
       </c>
-      <c r="J3" s="68" t="s">
+      <c r="J3" s="69" t="s">
         <v>86</v>
       </c>
-      <c r="K3" s="68" t="s">
+      <c r="K3" s="69" t="s">
         <v>87</v>
       </c>
-      <c r="L3" s="68" t="s">
+      <c r="L3" s="69" t="s">
         <v>88</v>
       </c>
-      <c r="M3" s="68" t="s">
+      <c r="M3" s="69" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="68"/>
-      <c r="B4" s="68"/>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
+      <c r="A4" s="69"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
       <c r="E4" s="37" t="s">
         <v>89</v>
       </c>
@@ -3076,11 +3071,11 @@
       <c r="H4" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="I4" s="68"/>
-      <c r="J4" s="68"/>
-      <c r="K4" s="68"/>
-      <c r="L4" s="68"/>
-      <c r="M4" s="68"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="69"/>
+      <c r="K4" s="69"/>
+      <c r="L4" s="69"/>
+      <c r="M4" s="69"/>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="44" t="s">
@@ -3122,7 +3117,7 @@
       <c r="M5" s="39"/>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="45" t="s">
         <v>114</v>
       </c>
       <c r="B6" s="39" t="s">
@@ -3161,7 +3156,7 @@
       <c r="M6" s="39"/>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="45" t="s">
         <v>114</v>
       </c>
       <c r="B7" s="39" t="s">
@@ -3200,7 +3195,7 @@
       <c r="M7" s="39"/>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="45" t="s">
         <v>114</v>
       </c>
       <c r="B8" s="39" t="s">
@@ -3239,7 +3234,7 @@
       <c r="M8" s="39"/>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="45" t="s">
         <v>114</v>
       </c>
       <c r="B9" s="39" t="s">
@@ -3278,7 +3273,7 @@
       <c r="M9" s="39"/>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="45" t="s">
         <v>114</v>
       </c>
       <c r="B10" s="39" t="s">
@@ -3317,7 +3312,7 @@
       <c r="M10" s="39"/>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="44" t="s">
+      <c r="A11" s="45" t="s">
         <v>114</v>
       </c>
       <c r="B11" s="39" t="s">
@@ -3356,7 +3351,7 @@
       <c r="M11" s="39"/>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="45" t="s">
         <v>114</v>
       </c>
       <c r="B12" s="39" t="s">
@@ -3395,7 +3390,7 @@
       <c r="M12" s="39"/>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="45" t="s">
         <v>114</v>
       </c>
       <c r="B13" s="39" t="s">
@@ -3434,7 +3429,7 @@
       <c r="M13" s="39"/>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="44" t="s">
+      <c r="A14" s="45" t="s">
         <v>114</v>
       </c>
       <c r="B14" s="39" t="s">
@@ -3473,7 +3468,7 @@
       <c r="M14" s="39"/>
     </row>
     <row r="15" spans="1:13">
-      <c r="A15" s="44" t="s">
+      <c r="A15" s="45" t="s">
         <v>114</v>
       </c>
       <c r="B15" s="39" t="s">
@@ -3512,7 +3507,7 @@
       <c r="M15" s="39"/>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="44" t="s">
+      <c r="A16" s="45" t="s">
         <v>114</v>
       </c>
       <c r="B16" s="39" t="s">
@@ -3551,7 +3546,7 @@
       <c r="M16" s="39"/>
     </row>
     <row r="17" spans="1:13">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="45" t="s">
         <v>114</v>
       </c>
       <c r="B17" s="39" t="s">
@@ -3590,7 +3585,7 @@
       <c r="M17" s="39"/>
     </row>
     <row r="18" spans="1:13">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="45" t="s">
         <v>114</v>
       </c>
       <c r="B18" s="39" t="s">
@@ -3629,7 +3624,7 @@
       <c r="M18" s="39"/>
     </row>
     <row r="19" spans="1:13">
-      <c r="A19" s="44" t="s">
+      <c r="A19" s="45" t="s">
         <v>114</v>
       </c>
       <c r="B19" s="39" t="s">
@@ -3668,7 +3663,7 @@
       <c r="M19" s="39"/>
     </row>
     <row r="20" spans="1:13">
-      <c r="A20" s="44" t="s">
+      <c r="A20" s="45" t="s">
         <v>114</v>
       </c>
       <c r="B20" s="39" t="s">
@@ -3707,7 +3702,7 @@
       <c r="M20" s="39"/>
     </row>
     <row r="21" spans="1:13">
-      <c r="A21" s="44" t="s">
+      <c r="A21" s="45" t="s">
         <v>114</v>
       </c>
       <c r="B21" s="39" t="s">
@@ -3746,7 +3741,7 @@
       <c r="M21" s="39"/>
     </row>
     <row r="22" spans="1:13">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="45" t="s">
         <v>114</v>
       </c>
       <c r="B22" s="39" t="s">
@@ -3785,7 +3780,7 @@
       <c r="M22" s="39"/>
     </row>
     <row r="23" spans="1:13">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="45" t="s">
         <v>114</v>
       </c>
       <c r="B23" s="39" t="s">
@@ -3824,7 +3819,7 @@
       <c r="M23" s="39"/>
     </row>
     <row r="24" spans="1:13">
-      <c r="A24" s="44" t="s">
+      <c r="A24" s="45" t="s">
         <v>114</v>
       </c>
       <c r="B24" s="39" t="s">
@@ -3863,7 +3858,7 @@
       <c r="M24" s="39"/>
     </row>
     <row r="25" spans="1:13">
-      <c r="A25" s="44" t="s">
+      <c r="A25" s="45" t="s">
         <v>114</v>
       </c>
       <c r="B25" s="39" t="s">
@@ -3902,7 +3897,7 @@
       <c r="M25" s="39"/>
     </row>
     <row r="26" spans="1:13">
-      <c r="A26" s="44" t="s">
+      <c r="A26" s="45" t="s">
         <v>114</v>
       </c>
       <c r="B26" s="39" t="s">
@@ -3941,7 +3936,7 @@
       <c r="M26" s="39"/>
     </row>
     <row r="27" spans="1:13">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="45" t="s">
         <v>114</v>
       </c>
       <c r="B27" s="39" t="s">
@@ -3980,7 +3975,7 @@
       <c r="M27" s="39"/>
     </row>
     <row r="28" spans="1:13">
-      <c r="A28" s="44" t="s">
+      <c r="A28" s="45" t="s">
         <v>114</v>
       </c>
       <c r="B28" s="39" t="s">
@@ -4028,7 +4023,7 @@
       <c r="C29" s="39">
         <v>7</v>
       </c>
-      <c r="D29" s="69">
+      <c r="D29" s="46">
         <v>44136</v>
       </c>
       <c r="E29" s="41">
@@ -4067,7 +4062,7 @@
       <c r="C30" s="39">
         <v>7</v>
       </c>
-      <c r="D30" s="69">
+      <c r="D30" s="46">
         <v>44137</v>
       </c>
       <c r="E30" s="41">
@@ -4106,7 +4101,7 @@
       <c r="C31" s="39">
         <v>7</v>
       </c>
-      <c r="D31" s="69">
+      <c r="D31" s="46">
         <v>44138</v>
       </c>
       <c r="E31" s="41">
@@ -4145,7 +4140,7 @@
       <c r="C32" s="39">
         <v>7</v>
       </c>
-      <c r="D32" s="69">
+      <c r="D32" s="46">
         <v>44139</v>
       </c>
       <c r="E32" s="41">
@@ -4184,7 +4179,7 @@
       <c r="C33" s="39">
         <v>7</v>
       </c>
-      <c r="D33" s="69">
+      <c r="D33" s="46">
         <v>44140</v>
       </c>
       <c r="E33" s="41">
@@ -4223,7 +4218,7 @@
       <c r="C34" s="39">
         <v>7</v>
       </c>
-      <c r="D34" s="69">
+      <c r="D34" s="46">
         <v>44141</v>
       </c>
       <c r="E34" s="41">
@@ -4262,7 +4257,7 @@
       <c r="C35" s="39">
         <v>7</v>
       </c>
-      <c r="D35" s="69">
+      <c r="D35" s="46">
         <v>44142</v>
       </c>
       <c r="E35" s="41">
@@ -4301,7 +4296,7 @@
       <c r="C36" s="39">
         <v>7</v>
       </c>
-      <c r="D36" s="69">
+      <c r="D36" s="46">
         <v>44143</v>
       </c>
       <c r="E36" s="41">
@@ -4340,7 +4335,7 @@
       <c r="C37" s="39">
         <v>7</v>
       </c>
-      <c r="D37" s="69">
+      <c r="D37" s="46">
         <v>44144</v>
       </c>
       <c r="E37" s="41">
@@ -4379,7 +4374,7 @@
       <c r="C38" s="39">
         <v>7</v>
       </c>
-      <c r="D38" s="69">
+      <c r="D38" s="46">
         <v>44145</v>
       </c>
       <c r="E38" s="41">
@@ -4418,7 +4413,7 @@
       <c r="C39" s="39">
         <v>7</v>
       </c>
-      <c r="D39" s="69">
+      <c r="D39" s="46">
         <v>44146</v>
       </c>
       <c r="E39" s="41">
@@ -4457,7 +4452,7 @@
       <c r="C40" s="39">
         <v>7</v>
       </c>
-      <c r="D40" s="69">
+      <c r="D40" s="46">
         <v>44147</v>
       </c>
       <c r="E40" s="41">
@@ -4496,7 +4491,7 @@
       <c r="C41" s="39">
         <v>7</v>
       </c>
-      <c r="D41" s="69">
+      <c r="D41" s="46">
         <v>44148</v>
       </c>
       <c r="E41" s="41">
@@ -4535,7 +4530,7 @@
       <c r="C42" s="39">
         <v>7</v>
       </c>
-      <c r="D42" s="69">
+      <c r="D42" s="46">
         <v>44149</v>
       </c>
       <c r="E42" s="41">
@@ -4574,7 +4569,7 @@
       <c r="C43" s="39">
         <v>7</v>
       </c>
-      <c r="D43" s="69">
+      <c r="D43" s="46">
         <v>44150</v>
       </c>
       <c r="E43" s="41">
@@ -4613,7 +4608,7 @@
       <c r="C44" s="39">
         <v>7</v>
       </c>
-      <c r="D44" s="69">
+      <c r="D44" s="46">
         <v>44151</v>
       </c>
       <c r="E44" s="41">
@@ -4652,7 +4647,7 @@
       <c r="C45" s="39">
         <v>7</v>
       </c>
-      <c r="D45" s="69">
+      <c r="D45" s="46">
         <v>44152</v>
       </c>
       <c r="E45" s="41">
@@ -4691,7 +4686,7 @@
       <c r="C46" s="39">
         <v>7</v>
       </c>
-      <c r="D46" s="69">
+      <c r="D46" s="46">
         <v>44153</v>
       </c>
       <c r="E46" s="41">
@@ -4730,7 +4725,7 @@
       <c r="C47" s="39">
         <v>7</v>
       </c>
-      <c r="D47" s="69">
+      <c r="D47" s="46">
         <v>44154</v>
       </c>
       <c r="E47" s="41">
@@ -4769,7 +4764,7 @@
       <c r="C48" s="39">
         <v>7</v>
       </c>
-      <c r="D48" s="69">
+      <c r="D48" s="46">
         <v>44155</v>
       </c>
       <c r="E48" s="41">
@@ -4808,7 +4803,7 @@
       <c r="C49" s="39">
         <v>7</v>
       </c>
-      <c r="D49" s="69">
+      <c r="D49" s="46">
         <v>44156</v>
       </c>
       <c r="E49" s="41">
@@ -4847,7 +4842,7 @@
       <c r="C50" s="39">
         <v>7</v>
       </c>
-      <c r="D50" s="69">
+      <c r="D50" s="46">
         <v>44157</v>
       </c>
       <c r="E50" s="41">
@@ -4886,7 +4881,7 @@
       <c r="C51" s="39">
         <v>7</v>
       </c>
-      <c r="D51" s="69">
+      <c r="D51" s="46">
         <v>44158</v>
       </c>
       <c r="E51" s="41">
@@ -4925,7 +4920,7 @@
       <c r="C52" s="39">
         <v>7</v>
       </c>
-      <c r="D52" s="69">
+      <c r="D52" s="46">
         <v>44159</v>
       </c>
       <c r="E52" s="41">

</xml_diff>